<commit_message>
working mobile rev 1.0
</commit_message>
<xml_diff>
--- a/assets/data/Data_Riesgo_MANUAL.xlsx
+++ b/assets/data/Data_Riesgo_MANUAL.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="31ene2022" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="10jul2022" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="10jun2022" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -755,7 +756,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
         <v>0.7425983231166966</v>
@@ -1360,4 +1361,475 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Point</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Riesgo</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>NDVI</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Latitud</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Longitud</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.8354177186702311</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6.15818348129518</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-75.78945109963882</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.8054641585934869</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6.158839773883416</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-75.78945109963882</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.7842966904325106</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6.159496066471652</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-75.78945109963882</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.8078793282470147</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6.160152359059888</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-75.78945109963882</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.7468479526476191</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6.160808651648123</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-75.78945109963882</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.6688650456038993</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6.15818348129518</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-75.7885922824137</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.803323712101627</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6.158839773883416</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-75.7885922824137</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.7724477892480791</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6.159496066471652</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-75.7885922824137</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.8173297342579228</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6.160152359059888</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-75.7885922824137</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8754531743872137</v>
+      </c>
+      <c r="D11" t="n">
+        <v>6.160808651648123</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-75.7885922824137</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.6657485699358098</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6.15818348129518</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-75.78773346518857</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8600671006557239</v>
+      </c>
+      <c r="D13" t="n">
+        <v>6.158839773883416</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-75.78773346518857</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8757465203616336</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6.159496066471652</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-75.78773346518857</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.8046835140365085</v>
+      </c>
+      <c r="D15" t="n">
+        <v>6.160152359059888</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-75.78773346518857</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8830674665163043</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6.160808651648123</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-75.78773346518857</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.4625837282354751</v>
+      </c>
+      <c r="D17" t="n">
+        <v>6.15818348129518</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-75.78687464796343</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.7907732269250011</v>
+      </c>
+      <c r="D18" t="n">
+        <v>6.158839773883416</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-75.78687464796343</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.7704232451339251</v>
+      </c>
+      <c r="D19" t="n">
+        <v>6.159496066471652</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-75.78687464796343</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.804655329489094</v>
+      </c>
+      <c r="D20" t="n">
+        <v>6.160152359059888</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-75.78687464796343</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.875232071071354</v>
+      </c>
+      <c r="D21" t="n">
+        <v>6.160808651648123</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-75.78687464796343</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.4250888714528885</v>
+      </c>
+      <c r="D22" t="n">
+        <v>6.15818348129518</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-75.78601583073831</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.5670474935648414</v>
+      </c>
+      <c r="D23" t="n">
+        <v>6.158839773883416</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-75.78601583073831</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.2676151827328355</v>
+      </c>
+      <c r="D24" t="n">
+        <v>6.159496066471652</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-75.78601583073831</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.7720649349443865</v>
+      </c>
+      <c r="D25" t="n">
+        <v>6.160152359059888</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-75.78601583073831</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.8234034213899299</v>
+      </c>
+      <c r="D26" t="n">
+        <v>6.160808651648123</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-75.78601583073831</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>